<commit_message>
Update report of Cublas
added final version of cublas report
</commit_message>
<xml_diff>
--- a/reportCublas.xlsx
+++ b/reportCublas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=META-INF/manifest.xml><?xml version="1.0" encoding="utf-8"?>
-<manifest:manifest xmlns:manifest="urn:oasis:names:tc:opendocument:xmlns:manifest:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" manifest:version="1.2">
-  <manifest:file-entry manifest:full-path="/" manifest:version="1.2" manifest:media-type="application/vnd.oasis.opendocument.spreadsheet"/>
+<manifest:manifest xmlns:manifest="urn:oasis:names:tc:opendocument:xmlns:manifest:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" manifest:version="1.3">
+  <manifest:file-entry manifest:full-path="/" manifest:version="1.3" manifest:media-type="application/vnd.oasis.opendocument.spreadsheet"/>
   <manifest:file-entry manifest:full-path="Configurations2/" manifest:media-type="application/vnd.sun.xml.ui.configuration"/>
   <manifest:file-entry manifest:full-path="manifest.rdf" manifest:media-type="application/rdf+xml"/>
   <manifest:file-entry manifest:full-path="styles.xml" manifest:media-type="text/xml"/>
@@ -13,10 +13,11 @@
 </file>
 
 <file path=content.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-content xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:rpt="http://openoffice.org/2005/report" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xforms="http://www.w3.org/2002/xforms" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" office:version="1.2">
+<office:document-content xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:rpt="http://openoffice.org/2005/report" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xforms="http://www.w3.org/2002/xforms" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" office:version="1.3">
   <office:scripts/>
   <office:font-face-decls>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
+    <style:font-face style:name="Arial" svg:font-family="Arial" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Lucida Sans" svg:font-family="'Lucida Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Microsoft YaHei" svg:font-family="'Microsoft YaHei'" style:font-family-generic="system" style:font-pitch="variable"/>
   </office:font-face-decls>
@@ -25,96 +26,122 @@
       <style:table-column-properties fo:break-before="auto" style:column-width="2.258cm"/>
     </style:style>
     <style:style style:name="co2" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="2.94cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="1.988cm"/>
     </style:style>
     <style:style style:name="co3" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="7.96cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.069cm"/>
     </style:style>
     <style:style style:name="co4" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="2.286cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="13.208cm"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
       <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
-    </style:style>
-    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
-      <style:text-properties style:text-underline-style="none"/>
     </style:style>
     <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false"/>
       <style:paragraph-properties fo:text-align="start" fo:margin-left="0cm"/>
+    </style:style>
+    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties style:text-underline-style="none"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
     <office:spreadsheet>
       <table:calculation-settings table:automatic-find-labels="false" table:use-regular-expressions="false" table:use-wildcards="true"/>
       <table:table table:name="Лист1" table:style-name="ta1">
-        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="2" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co3" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co4" table:default-cell-style-name="ce2"/>
-        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>cublas</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+        <table:table-column table:style-name="co4" table:default-cell-style-name="Default"/>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Cublas </text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
             <text:p>GPU</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>значения в таблице усреднены для 10 тестов </text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="Default" office:value-type="string" calcext:value-type="string">
-            <text:p>openacc</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>GPU</text:p>
-          </table:table-cell>
+            <text:p>OpenACC</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="float" office:value="128" calcext:value-type="float">
             <text:p>128</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>~0,7693678с</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>~0,404</text:p>
-          </table:table-cell>
+            <text:p>~1,05с</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>~0,4c</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="128" calcext:value-type="float">
+            <text:p>128</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="float" office:value="256" calcext:value-type="float">
             <text:p>256</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>~1.658992837с</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>~4,768</text:p>
-          </table:table-cell>
+            <text:p>~1,93с</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>~4,8c</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="256" calcext:value-type="float">
+            <text:p>256</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="float" office:value="512" calcext:value-type="float">
             <text:p>512</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>~1.967320230с</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
+            <text:p>~4,1с</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>~6,7c</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="512" calcext:value-type="float">
+            <text:p>512</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="float" office:value="1024" calcext:value-type="float">
             <text:p>1024</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>~18.2091843274с</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce1"/>
-          <table:table-cell table:number-columns-repeated="2"/>
+            <text:p>~29,79с</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+            <text:p>~31,9c</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="1024" calcext:value-type="float">
+            <text:p>1024</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="5"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="4"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Примечание 1: значения в таблице усреднены для 10 тестов </text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="4"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Примечание 2: под OpenACC подразумевается оптимизированная программа </text:p>
+          </table:table-cell>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -124,33 +151,33 @@
 </file>
 
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-meta xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" office:version="1.2">
+<office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" office:version="1.3">
   <office:meta>
     <meta:creation-date>2022-04-21T09:42:55.601000000</meta:creation-date>
-    <meta:generator>LibreOffice/6.4.5.2$Windows_X86_64 LibreOffice_project/a726b36747cf2001e06b58ad5db1aa3a9a1872d6</meta:generator>
-    <dc:date>2022-05-19T12:22:52.377000000</dc:date>
-    <meta:editing-duration>PT31M47S</meta:editing-duration>
-    <meta:editing-cycles>2</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="15" meta:object-count="0"/>
+    <meta:generator>LibreOffice/7.1.2.2$Windows_X86_64 LibreOffice_project/8a45595d069ef5570103caea1b71cc9d82b2aae4</meta:generator>
+    <dc:date>2022-05-25T20:39:20.287000000</dc:date>
+    <meta:editing-duration>PT46M4S</meta:editing-duration>
+    <meta:editing-cycles>3</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="22" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
 
 <file path=settings.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-settings xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" office:version="1.2">
+<office:document-settings xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" office:version="1.3">
   <office:settings>
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">17702</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">2257</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">21780</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">3612</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Лист1">
               <config:config-item config:name="CursorPositionX" config:type="int">4</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">6</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">9</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -168,7 +195,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Лист1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1360</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1301</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -202,10 +229,10 @@
       <config:config-item config:name="GridColor" config:type="int">12632256</config:config-item>
       <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
       <config:config-item config:name="IsKernAsianPunctuation" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="IsOutlineSymbolsSet" config:type="boolean">true</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="EmbedLatinScriptFonts" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="IsOutlineSymbolsSet" config:type="boolean">true</config:config-item>
       <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
@@ -215,8 +242,8 @@
       <config:config-item config:name="IsRasterAxisSynchronized" config:type="boolean">true</config:config-item>
       <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string">PDF24</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">JQX+/1BERjI0AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUERGMjQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAEAQgQAAAAAAAAEAAhSAAAEdAAAM1ROVwAAAAAKAFAARABGADIANAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABBAMG3ABcA1PvgAEBAAkAmgs0CGQAAQAPAFgCAgABAFgCAgABAEEANAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAQAAAAIAAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABQUklWQjAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGAAAAAAAECcQJxAnAAAQJwAAAAAAAAAAaABcAwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAMAAAAAAAAAAAAQAFA0AwAoiAQAAAAAAAAAAAAAAAEAAAAAAAAAAAAAAAAAAAAAAB8bFJwDAAAABgAOAP8AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABoAAAAU01USgAAAAAQAFgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABIAQ09NUEFUX0RVUExFWF9NT0RFEwBEdXBsZXhNb2RlOjpVbmtub3du</config:config-item>
+      <config:config-item config:name="PrinterName" config:type="string">HP LaserJet MFP M227-M231</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">+jT+/0hQIExhc2VySmV0IE1GUCBNMjI3LU0yMzEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAASFAgTGFzZXJKZXQgTUZQIE0yMjctTTIzMSBQQ0wtNgAWAAEAFjQAAAAAAQAEAAhSAAAEdAAAM1ROVwAAAAAKAEgAUAAgAEwAYQBzAGUAcgBKAGUAdAAgAE0ARgBQACAATQAyADIANwAtAE0AMgAzADEAAAAAAAAAAAAAAAAAAAABBAMG3AAwM0O/AQIBAAkAmgs0CGQAAQADAVgCAQACAFgCAwABAEEANAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAQAAAAIAAAASAQAA/////0dJUzQAAAAAAAAAAAAAAABESU5VIgAIBmQIzCoJSwg/AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAC0AAAABAAAAZgAAAAAAAAABAAAAAgAAAAYAAAAAAAEAAQAAAAAAAAAAAAAAAQAAAAAAAAAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAACAYAAFNNVEoAAAAAEAD4BXsAMABiAGYAYQA1AGMAYgAwAC0AOQAzADkAMQAtADQAYQA2AGIALQBiADAAMABhAC0AMQBmADQAZQBiADYANwA5ADkANwBhADkAfQAAAElucHV0QmluAFVzZVByaW50ZXJTZXR0aW5nAFJFU0RMTABVbmlyZXNETEwATG9jYWxlAFJ1c3NpYW4AU3RyaW5nc0NsdXN0ZXIwAElEU19BQk9VVFRBQl9OQU1FAFN0cmluZ3NDbHVzdGVyMQBJRFNfQUJPVVRfSFBfQ09QWVJJR0hUMQBQcmludFF1YWxpdHkASGlnaABVc2VyUmVzb2x1dGlvbgBSZXNvbHV0aW9uRmFzdDEyMDAAUmVzb2x1dGlvbgA2MDBkcGkARG9jdW1lbnROdWxsU3RyaXBTa2lwcGluZwBTa2lwQWZ0ZXJDb250ZW50AENvbG9yTW9kZQBNb25vY2hyb21lAFBhcGVyU2l6ZQBBNABPcmllbnRhdGlvbgBQT1JUUkFJVABNZWRpYVR5cGUAQXV0b1NlbGVjdE1lZGlhVHlwZQBQcmludGVySW5pdGlhbGl6YXRpb24ARE9ORQBEdXBsZXgAVkVSVElDQUwATWFudWFsRHVwbGV4AE1hbnVhbFNpbXBsZXgASm9iRmxpcFBhZ2VVcABmYWxzZQBEb2N1bWVudE5VcAAxAE5VcEJvcmRlcnMAT2ZmAFByZXNlbnRhdGlvbkRpcmVjdGlvbgBSaWdodEJvdHRvbQBDb2xsYXRlAE9OAFBhZ2VSb3RhdGUxODAATm9Sb3RhdGlvbgBKb2JQYWdlT3JkZXIAU3RhbmRhcmQARG9jdW1lbnRFY29ub01vZGUAZmFsc2UARG9jdW1lbnRIeWJyaWRSYXN0ZXIASHlicmlkUmFzdGVyQXV0bwBEb2N1bWVudEVuYWJsZUJpZ0RhdGFDb2xsZWN0aW9uAEJpZ0RhdGFDb2xsZWN0aW9uT24ARG9jdW1lbnRJbnNlcnRQYWdlcwBOb0luc2VydFBhZ2VzAERvY3VtZW50QmxhbmtTaGVldEV4Y2VwdGlvbjEAQmVmb3JlRXhjZXB0aW9uUGFnZXMARG9jdW1lbnRCbGFua1NoZWV0RXhjZXB0aW9uMgBCZWZvcmVFeGNlcHRpb25QYWdlcwBEb2N1bWVudE1lZGlhRXhjZXB0aW9uMQBNZWRpYUV4Y2VwdGlvbjEARG9jdW1lbnRNZWRpYUV4Y2VwdGlvbjIATWVkaWFFeGNlcHRpb24yAERvY3VtZW50RXhjZXB0aW9uVXNhZ2UAU3BlY2lmaWVkUGFnZXMAUGFnZUJsYWNrVGV4dABOb25lAEdVSVN0cmluZ3MASURTX1VTRV9QQVBFUl9TSVpFAERvY3VtZW50Q292ZXJGcm9udABOb0NvdmVyAERvY3VtZW50Q292ZXJCYWNrAE5vQ292ZXIARG9jdW1lbnRJbnRlcmxlYXZlcwBOb0ludGVybGVhdmVzAFBhZ2VXYXRlcm1hcmsAVGV4dABQYWdlV2F0ZXJtYXJrUGxhY2VtZW50AENlbnRlcgBQYWdlV2F0ZXJtYXJrTGF5ZXJpbmcAT3ZlcmxheQBQYWdlV2F0ZXJtYXJrVXNhZ2UAQWxsUGFnZXMAUGFnZVBvc3RlcgAxAERvY3VtZW50QmluZGluZwBOT05FAFBhZ2VTY2FsaW5nAE5PTkUAU2NhbGVPZmZzZXRBbGlnbm1lbnQAQ2VudGVyAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAADMKgAAVjRETQEAAAAAAAAAWd9NkxwAAACUDgAAPgAAALBc+guRk2tKsAofTrZ5l6l4DgAA/AMAAAQAAACAAAAAAAAAAAAAAAABAAAABAAAAA4AAACAAAAAAQAAAAQAAAAYAAAAhAAAAAEAAAAEAAAAJgAAAIgAAAABAAAABAAAAEQAAACMAAAAAQAAAAQAAABkAAAAkAAAAAMAAAB+AAAAjAAAAJQAAAABAAAABAAAALQAAAAUAQAAAQAAAAQAAADmAAAAGAEAAAMAAAB+AAAAGgEAABwBAAADAAAAfgAAAEIBAACcAQAAAwAAAH4AAABoAQAAHAIAAAEAAAAEAAAAjgEAAJwCAAABAAAABAAAAL4BAACgAgAAAwAAAH4AAADwAQAApAIAAAMAAAB+AAAAFgIAACQDAAADAAAAfgAAADoCAACkAwAAAQAAAAQAAABkAgAAJAQAAAEAAAAEAAAAmAIAACgEAAADAAAAfgAAAM4CAAAsBAAAAwAAAH4AAAD4AgAArAQAAAMAAAB+AAAAIAMAACwFAAABAAAABAAAAFQDAACsBQAAAQAAAAQAAACSAwAAsAUAAAMAAAB+AAAA0gMAALQFAAADAAAAfgAAAAYEAAA0BgAAAwAAAH4AAAA4BAAAtAYAAAMAAAAAAQAAdgQAADQHAAADAAAAfgAAAKAEAAA0CAAAAQAAAAQAAADUBAAAtAgAAAEAAAAEAAAAEgUAALgIAAADAAAAfgAAAFIFAAC8CAAAAwAAAH4AAACGBQAAPAkAAAMAAAB+AAAAuAUAALwJAAADAAAAAAEAAPYFAAA8CgAAAwAAAAABAAAgBgAAPAsAAAEAAAAEAAAAQAYAADwMAAABAAAABAAAAGoGAABADAAAAQAAAAQAAACWBgAARAwAAAEAAAAEAAAAsgYAAEgMAAADAAAAAAIAANAGAABMDAAAAQAAAAQAAAD2BgAATA4AAAEAAAAEAAAAOgcAAFAOAAABAAAABAAAAIAHAABUDgAAAwAAAAACAAC0BwAAWA4AAAEAAAAEAAAA4gcAAFgQAAABAAAABAAAABYIAABcEAAAAwAAABIAAABECAAAYBAAAAMAAAAAAQAAcggAAHQQAAABAAAABAAAAKAIAAB0EQAAAQAAAAQAAADSCAAAeBEAAAEAAAAEAAAA/ggAAHwRAAABAAAABAAAAC4JAACAEQAAAwAAADAIAABoCQAAhBEAAAEAAAAEAAAAmAkAALQZAAABAAAABAAAANIJAAC4GQAAAwAAAIAAAAAOCgAAvBkAAAMAAACAAAAAHgoAADwaAAADAAAAGgAAADAKAAC8GgAAAwAAAAABAAA4CgAA2BoAAAMAAABAAAAASgoAANgbAAADAAAAIAAAAGQKAAAYHAAAYgBBAHIAcgBhAHkAAABaAG8AbwBtAAAAUABvAHMAdABlAHIAAABOAFUAcABCAG8AcgBkAGUAcgBXAGkAZAB0AGgAAABOAFUAcABCAG8AcgBkAGUAcgBMAGUAbgBnAHQAaAAAAE4AVQBwAEIAbwByAGQAZQByAEQAYQBzAGgATABlAG4AZwB0AGgAAABGAHIAbwBuAHQAQwBvAHYAZQByAE0AZQBkAGkAYQBTAGkAegBlAAAARgByAG8AbgB0AEMAbwB2AGUAcgBNAGUAZABpAGEAUwBpAHoAZQBXAGkAZAB0AGgAAABGAHIAbwBuAHQAQwBvAHYAZQByAE0AZQBkAGkAYQBTAGkAegBlAEgAZQBpAGcAaAB0AAAARgByAG8AbgB0AEMAbwB2AGUAcgBNAGUAZABpAGEAVAB5AHAAZQAAAEYAcgBvAG4AdABDAG8AdgBlAHIASQBuAHAAdQB0AEIAaQBuAAAAQgBhAGMAawBDAG8AdgBlAHIATQBlAGQAaQBhAFMAaQB6AGUAAABCAGEAYwBrAEMAbwB2AGUAcgBNAGUAZABpAGEAUwBpAHoAZQBXAGkAZAB0AGgAAABCAGEAYwBrAEMAbwB2AGUAcgBNAGUAZABpAGEAUwBpAHoAZQBIAGUAaQBnAGgAdAAAAEIAYQBjAGsAQwBvAHYAZQByAE0AZQBkAGkAYQBUAHkAcABlAAAAQgBhAGMAawBDAG8AdgBlAHIASQBuAHAAdQB0AEIAaQBuAAAASQBuAHQAZQByAGwAZQBhAHYAZQBzAE0AZQBkAGkAYQBTAGkAegBlAAAASQBuAHQAZQByAGwAZQBhAHYAZQBzAE0AZQBkAGkAYQBTAGkAegBlAFcAaQBkAHQAaAAAAEkAbgB0AGUAcgBsAGUAYQB2AGUAcwBNAGUAZABpAGEAUwBpAHoAZQBIAGUAaQBnAGgAdAAAAEkAbgB0AGUAcgBsAGUAYQB2AGUAcwBNAGUAZABpAGEAVAB5AHAAZQAAAEkAbgB0AGUAcgBsAGUAYQB2AGUAcwBJAG4AcAB1AHQAQgBpAG4AAABJAG4AcwBlAHIAdABFAG0AcAB0AHkAUABhAGcAZQBzAE0AZQBkAGkAYQBTAGkAegBlAAAASQBuAHMAZQByAHQARQBtAHAAdAB5AFAAYQBnAGUAcwBNAGUAZABpAGEAUwBpAHoAZQBXAGkAZAB0AGgAAABJAG4AcwBlAHIAdABFAG0AcAB0AHkAUABhAGcAZQBzAE0AZQBkAGkAYQBTAGkAegBlAEgAZQBpAGcAaAB0AAAASQBuAHMAZQByAHQARQBtAHAAdAB5AFAAYQBnAGUAcwBNAGUAZABpAGEAVAB5AHAAZQAAAEkAbgBzAGUAcgB0AEUAbQBwAHQAeQBQAGEAZwBlAHMASQBuAHAAdQB0AEIAaQBuAAAASQBuAHMAZQByAHQARQBtAHAAdAB5AFAAYQBnAGUAcwBFAHgAYwBlAHAAdABpAG8AbgBVAHMAYQBnAGUAAABJAG4AcwBlAHIAdABFAG0AcAB0AHkAUABhAGcAZQBzAEwAaQBzAHQAAABJAG4AcwBlAHIAdABQAHIAaQBuAHQAUABhAGcAZQBzAE0AZQBkAGkAYQBTAGkAegBlAAAASQBuAHMAZQByAHQAUAByAGkAbgB0AFAAYQBnAGUAcwBNAGUAZABpAGEAUwBpAHoAZQBXAGkAZAB0AGgAAABJAG4AcwBlAHIAdABQAHIAaQBuAHQAUABhAGcAZQBzAE0AZQBkAGkAYQBTAGkAegBlAEgAZQBpAGcAaAB0AAAASQBuAHMAZQByAHQAUAByAGkAbgB0AFAAYQBnAGUAcwBNAGUAZABpAGEAVAB5AHAAZQAAAEkAbgBzAGUAcgB0AFAAcgBpAG4AdABQAGEAZwBlAHMASQBuAHAAdQB0AEIAaQBuAAAASQBuAHMAZQByAHQAUAByAGkAbgB0AFAAYQBnAGUAcwBFAHgAYwBlAHAAdABpAG8AbgBVAHMAYQBnAGUAAABJAG4AcwBlAHIAdABQAHIAaQBuAHQAUABhAGcAZQBzAEwAaQBzAHQAAABUAGEAcgBnAGUAdABNAGUAZABpAGEAUwBpAHoAZQAAAFQAYQByAGcAZQB0AE0AZQBkAGkAYQBTAGkAegBlAFcAaQBkAHQAaAAAAFQAYQByAGcAZQB0AE0AZQBkAGkAYQBTAGkAegBlAEgAZQBpAGcAaAB0AAAAQgBpAG4AZABpAG4AZwBHAHUAdAB0AGUAcgAAAFMAaQBnAG4AYQB0AHUAcgBlAFAAYQBnAGUAcwAAAFAAYQBnAGUAVwBhAHQAZQByAG0AYQByAGsATgBhAG0AZQBIAAAAUABhAGcAZQBXAGEAdABlAHIAbQBhAHIAawBQAGwAYQBjAGUAbQBlAG4AdABPAGYAZgBzAGUAdABXAGkAZAB0AGgAAABQAGEAZwBlAFcAYQB0AGUAcgBtAGEAcgBrAFAAbABhAGMAZQBtAGUAbgB0AE8AZgBmAHMAZQB0AEgAZQBpAGcAaAB0AAAAUABhAGcAZQBXAGEAdABlAHIAbQBhAHIAawBUAHIAYQBuAHMAcABhAHIAZQBuAGMAeQAAAFAAYQBnAGUAVwBhAHQAZQByAG0AYQByAGsAVABlAHgAdABUAGUAeAB0AEgAAABQAGEAZwBlAFcAYQB0AGUAcgBtAGEAcgBrAFQAZQB4AHQARgBvAG4AdABTAGkAegBlAAAAUABhAGcAZQBXAGEAdABlAHIAbQBhAHIAawBUAGUAeAB0AEEAbgBnAGwAZQAAAFAAYQBnAGUAVwBhAHQAZQByAG0AYQByAGsAVABlAHgAdABDAG8AbABvAHIAAABQAGEAZwBlAFcAYQB0AGUAcgBtAGEAcgBrAFQAZQB4AHQARgBvAG4AdABIAAAAUABhAGcAZQBXAGEAdABlAHIAbQBhAHIAawBUAGUAeAB0AE8AdQB0AGwAaQBuAGUAAABQAGEAZwBlAFcAYQB0AGUAcgBtAGEAcgBrAFQAZQB4AHQAQgBvAGwAZAAAAFAAYQBnAGUAVwBhAHQAZQByAG0AYQByAGsAVABlAHgAdABJAHQAYQBsAGkAYwAAAFAAYQBnAGUAVwBhAHQAZQByAG0AYQByAGsAVABlAHgAdABSAGkAZwBoAHQAVABvAEwAZQBmAHQAAABQAGEAZwBlAFcAYQB0AGUAcgBtAGEAcgBrAEkAbQBhAGcAZQBGAGkAbABlAEgAAABQAGEAZwBlAFcAYQB0AGUAcgBtAGEAcgBrAEkAbQBhAGcAZQBTAGMAYQBsAGUAVwBpAGQAdABoAAAAUABhAGcAZQBXAGEAdABlAHIAbQBhAHIAawBJAG0AYQBnAGUAUwBjAGEAbABlAEgAZQBpAGcAaAB0AAAASgBvAGIATgBhAG0AZQAAAFUAcwBlAHIATgBhAG0AZQAAAFAASQBOAAAAUABhAHMAcwB3AG8AcgBkAAAAUwBoAG8AcgB0AGMAdQB0AE4AYQBtAGUAAABEAHUAcABsAGUAeABNAG8AZABlAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGQAAAABAAAAAAAAAAAAAAAAAAAAbgBzADAAMAAwADAAOgBVAHMAZQBQAGEAZwBlAE0AZQBkAGkAYQBTAGkAegBlAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAHAAcwBrADoAUABsAGEAaQBuAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAcABzAGsAOgBBAHUAdABvAFMAZQBsAGUAYwB0AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABuAHMAMAAwADAAMAA6AFUAcwBlAFAAYQBnAGUATQBlAGQAaQBhAFMAaQB6AGUAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAcABzAGsAOgBQAGwAYQBpAG4AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABwAHMAawA6AEEAdQB0AG8AUwBlAGwAZQBjAHQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAG4AcwAwADAAMAAwADoAVQBzAGUAUABhAGcAZQBNAGUAZABpAGEAUwBpAHoAZQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABwAHMAawA6AFAAbABhAGkAbgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAHAAcwBrADoAQQB1AHQAbwBTAGUAbABlAGMAdAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAbgBzADAAMAAwADAAOgBVAHMAZQBQAGEAZwBlAE0AZQBkAGkAYQBTAGkAegBlAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAHAAcwBrADoAQQB1AHQAbwBTAGUAbABlAGMAdAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAcABzAGsAOgBBAHUAdABvAFMAZQBsAGUAYwB0AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABuAHMAMAAwADAAMAA6AFMAcABlAGMAaQBmAGkAZQBkAFAAYQBnAGUAcwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABuAHMAMAAwADAAMAA6AFUAcwBlAFAAYQBnAGUATQBlAGQAaQBhAFMAaQB6AGUAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAcABzAGsAOgBBAHUAdABvAFMAZQBsAGUAYwB0AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABwAHMAawA6AEEAdQB0AG8AUwBlAGwAZQBjAHQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAG4AcwAwADAAMAAwADoAUwBwAGUAYwBpAGYAaQBlAGQAUABhAGcAZQBzAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAADIAAAAwADAANgAxAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEgAAAAAAAAARgBGAEYARgAwADAAMAAwAAAAAAAwADAANgAxAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAADAAMAA0ADEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAGQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQQB1AHQAbwBtAGEAdABpAGMAAAAAAAAAAAAAAAAAAAASAENPTVBBVF9EVVBMRVhfTU9ERRQARHVwbGV4TW9kZTo6TG9uZ0VkZ2U=</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
       <config:config-item config:name="SaveThumbnail" config:type="boolean">true</config:config-item>
       <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
@@ -229,15 +256,21 @@
       <config:config-item config:name="EmbedOnlyUsedFonts" config:type="boolean">false</config:config-item>
       <config:config-item config:name="EmbedAsianScriptFonts" config:type="boolean">true</config:config-item>
       <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
+      <config:config-item-map-named config:name="ScriptConfiguration">
+        <config:config-item-map-entry config:name="Лист1">
+          <config:config-item config:name="CodeName" config:type="string">Лист1</config:config-item>
+        </config:config-item-map-entry>
+      </config:config-item-map-named>
     </config:config-item-set>
   </office:settings>
 </office:document-settings>
 </file>
 
 <file path=styles.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-styles xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:rpt="http://openoffice.org/2005/report" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" office:version="1.2">
+<office:document-styles xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:rpt="http://openoffice.org/2005/report" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" office:version="1.3">
   <office:font-face-decls>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
+    <style:font-face style:name="Arial" svg:font-family="Arial" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Lucida Sans" svg:font-family="'Lucida Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Microsoft YaHei" svg:font-family="'Microsoft YaHei'" style:font-family-generic="system" style:font-pitch="variable"/>
   </office:font-face-decls>
@@ -250,13 +283,13 @@
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
     <style:style style:name="Default" style:family="table-cell"/>
-    <style:style style:name="Heading_20__28_user_29_" style:display-name="Heading (user)" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="Heading" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties fo:color="#000000" fo:font-size="24pt" fo:font-style="normal" fo:font-weight="bold"/>
     </style:style>
-    <style:style style:name="Heading_20_1" style:display-name="Heading 1" style:family="table-cell" style:parent-style-name="Heading_20__28_user_29_">
+    <style:style style:name="Heading_20_1" style:display-name="Heading 1" style:family="table-cell" style:parent-style-name="Heading">
       <style:text-properties fo:color="#000000" fo:font-size="18pt" fo:font-style="normal" fo:font-weight="normal"/>
     </style:style>
-    <style:style style:name="Heading_20_2" style:display-name="Heading 2" style:family="table-cell" style:parent-style-name="Heading_20__28_user_29_">
+    <style:style style:name="Heading_20_2" style:display-name="Heading 2" style:family="table-cell" style:parent-style-name="Heading">
       <style:text-properties fo:color="#000000" fo:font-size="12pt" fo:font-style="normal" fo:font-weight="normal"/>
     </style:style>
     <style:style style:name="Text" style:family="table-cell" style:parent-style-name="Default"/>
@@ -304,8 +337,14 @@
     <style:style style:name="Accent_20_3" style:display-name="Accent 3" style:family="table-cell" style:parent-style-name="Accent">
       <style:table-cell-properties fo:background-color="#dddddd"/>
     </style:style>
+    <style:style style:name="Result" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:color="#000000" fo:font-size="10pt" fo:font-style="italic" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="#000000" fo:font-weight="bold"/>
+    </style:style>
   </office:styles>
   <office:automatic-styles>
+    <number:number-style style:name="N2">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1"/>
+    </number:number-style>
     <style:page-layout style:name="Mpm1">
       <style:page-layout-properties style:writing-mode="lr-tb"/>
       <style:header-style>
@@ -358,9 +397,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2022-05-19">00.00.0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2022-05-25">00.00.0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="11:34:56.652000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="20:19:27.698000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>